<commit_message>
SHG Meetings class test
</commit_message>
<xml_diff>
--- a/SHG Rough.xlsx
+++ b/SHG Rough.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\eclipse-workspace\LokOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\eclipse-workspace\LokOSMain\XLS Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5B0A07-4D8D-4B5C-B7B4-4F94661EB8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402DA5D8-C953-4D2B-B2F6-59C03802D6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C04F3656-6872-4AAE-94DF-BF61196F368D}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="SHGs" sheetId="6" r:id="rId2"/>
     <sheet name="Members" sheetId="3" r:id="rId3"/>
     <sheet name="Web Login" sheetId="4" r:id="rId4"/>
+    <sheet name="Cutoff Meetings" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -350,7 +351,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="370">
   <si>
     <t>LokOS_2.0.31.apk</t>
   </si>
@@ -1057,83 +1058,416 @@
     <t>821 Re-Type Account Number</t>
   </si>
   <si>
-    <t>051, 027 Update</t>
+    <t>25_01_2016</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Co-opted</t>
+  </si>
+  <si>
+    <t>02_01_2012</t>
+  </si>
+  <si>
+    <t>05_06_2020</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>Special Class</t>
+  </si>
+  <si>
+    <t>Fortnightly</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Yes-External</t>
+  </si>
+  <si>
+    <t>#9455885271</t>
+  </si>
+  <si>
+    <t>Horticulture Activities</t>
+  </si>
+  <si>
+    <t>Other livestock rearing</t>
+  </si>
+  <si>
+    <t>NTFP Collection</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Aaryaman Gupta:9455120510</t>
+  </si>
+  <si>
+    <t>SBIN0000131</t>
+  </si>
+  <si>
+    <t>Main Branch</t>
+  </si>
+  <si>
+    <t>#40256541490</t>
+  </si>
+  <si>
+    <t>02_01_2022</t>
+  </si>
+  <si>
+    <t>New Members</t>
+  </si>
+  <si>
+    <t>Aaryaman Two</t>
+  </si>
+  <si>
+    <t>Aaryaman  Bannerji</t>
+  </si>
+  <si>
+    <t>Update SHG</t>
   </si>
   <si>
     <t>New SHG</t>
   </si>
   <si>
-    <t>Aaryama Three SHG</t>
-  </si>
-  <si>
-    <t>25_01_2016</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Co-opted</t>
-  </si>
-  <si>
-    <t>02_01_2012</t>
-  </si>
-  <si>
-    <t>05_06_2020</t>
-  </si>
-  <si>
-    <t>Special</t>
-  </si>
-  <si>
-    <t>OTHER</t>
-  </si>
-  <si>
-    <t>Special Class</t>
-  </si>
-  <si>
-    <t>Fortnightly</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Yes-External</t>
-  </si>
-  <si>
-    <t>#9455885271</t>
-  </si>
-  <si>
-    <t>Horticulture Activities</t>
-  </si>
-  <si>
-    <t>Other livestock rearing</t>
-  </si>
-  <si>
-    <t>NTFP Collection</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Aaryaman Gupta:9455120510</t>
-  </si>
-  <si>
-    <t>SBIN0000131</t>
-  </si>
-  <si>
-    <t>Main Branch</t>
-  </si>
-  <si>
-    <t>#40256541490</t>
-  </si>
-  <si>
-    <t>02_01_2022</t>
+    <t>Aaryaman Three SHG</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>051,023 Update</t>
+  </si>
+  <si>
+    <t>#40256541498</t>
+  </si>
+  <si>
+    <t>Aaryaman One SHG</t>
+  </si>
+  <si>
+    <t>Update MemberApprove SHG</t>
+  </si>
+  <si>
+    <t>5,20 Update</t>
+  </si>
+  <si>
+    <t>#40256541480</t>
+  </si>
+  <si>
+    <t>New Meeting Number</t>
+  </si>
+  <si>
+    <t>Meeting Date</t>
+  </si>
+  <si>
+    <t>001 Attendence</t>
+  </si>
+  <si>
+    <t>002 Compulsory Saving</t>
+  </si>
+  <si>
+    <t>003 Voluntary Saving</t>
+  </si>
+  <si>
+    <t>004 Number of Loans</t>
+  </si>
+  <si>
+    <t>005 Amount of Loans</t>
+  </si>
+  <si>
+    <t>006 Fund Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">106 Disbursed Loan Amount </t>
+  </si>
+  <si>
+    <t>206 Principal Repaid</t>
+  </si>
+  <si>
+    <t>007 Fund Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">107 Disbursed Loan Amount </t>
+  </si>
+  <si>
+    <t>207 Principal Repaid</t>
+  </si>
+  <si>
+    <t>008 Fund Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">108 Disbursed Loan Amount </t>
+  </si>
+  <si>
+    <t>208 Principal Repaid</t>
+  </si>
+  <si>
+    <t>009 Share Capital</t>
+  </si>
+  <si>
+    <t>010 Membership Fee</t>
+  </si>
+  <si>
+    <t>011 Investment At(Group Investment)</t>
+  </si>
+  <si>
+    <t>111 Type of Saving</t>
+  </si>
+  <si>
+    <t>211 Amount</t>
+  </si>
+  <si>
+    <t>012 Institution(Grp Closed Loan)</t>
+  </si>
+  <si>
+    <t>112 Borrowed From</t>
+  </si>
+  <si>
+    <t>212 Fund Source</t>
+  </si>
+  <si>
+    <t>312 Number of Loans</t>
+  </si>
+  <si>
+    <t>412 Total Amount</t>
+  </si>
+  <si>
+    <t>013 Institution(Grp Active Loan)</t>
+  </si>
+  <si>
+    <t>113 Borrowed From</t>
+  </si>
+  <si>
+    <t>213 Loan Account No.</t>
+  </si>
+  <si>
+    <t>313 Fund Source</t>
+  </si>
+  <si>
+    <t>413 Type of Loan</t>
+  </si>
+  <si>
+    <t>513 Loan Disbursement Date</t>
+  </si>
+  <si>
+    <t>1613 Repayment Frequency</t>
+  </si>
+  <si>
+    <t>014 Source(Fund Received)</t>
+  </si>
+  <si>
+    <t>114 Fund Source</t>
+  </si>
+  <si>
+    <t>214 Mode of Receipt</t>
+  </si>
+  <si>
+    <t>314 Total Amount Received</t>
+  </si>
+  <si>
+    <t>015 Cash in Hand(Grp Cash Balance)</t>
+  </si>
+  <si>
+    <t>115 Cash in Transit</t>
+  </si>
+  <si>
+    <t>215 Date of Balance Taken</t>
+  </si>
+  <si>
+    <t>016 Bank Name(Grp Bank Balance)</t>
+  </si>
+  <si>
+    <t>116 Cash in Bank</t>
+  </si>
+  <si>
+    <t>216 Cheque issued but amount not debited</t>
+  </si>
+  <si>
+    <t>316 Cheque received but amount not credited</t>
+  </si>
+  <si>
+    <t>416 Date of Balance taken</t>
+  </si>
+  <si>
+    <t>BALAJI MAHILA SHG</t>
+  </si>
+  <si>
+    <t>22_02_2022</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>04_07_2019</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>VO</t>
+  </si>
+  <si>
+    <t>Share Capital</t>
+  </si>
+  <si>
+    <t>CLF</t>
+  </si>
+  <si>
+    <t>306 PrincipalOutstandingIncludingArrears</t>
+  </si>
+  <si>
+    <t>406 PrincipalArrears</t>
+  </si>
+  <si>
+    <t>506 InterestRateAnnually</t>
+  </si>
+  <si>
+    <t>606 InterestPaid</t>
+  </si>
+  <si>
+    <t>706 OverdueInterest</t>
+  </si>
+  <si>
+    <t>806 TotalOverdue</t>
+  </si>
+  <si>
+    <t>906 LoanDisbursementDateDisbursement</t>
+  </si>
+  <si>
+    <t>1006 ModeofReceipt</t>
+  </si>
+  <si>
+    <t>1106 PeriodMonths</t>
+  </si>
+  <si>
+    <t>1206 LoanRepaymentFrequency</t>
+  </si>
+  <si>
+    <t>1306 Purpose</t>
+  </si>
+  <si>
+    <t>307 PrincipalOutstandingIncludingArrears</t>
+  </si>
+  <si>
+    <t>407 PrincipalArrears</t>
+  </si>
+  <si>
+    <t>507 InterestRateAnnually</t>
+  </si>
+  <si>
+    <t>607 InterestPaid</t>
+  </si>
+  <si>
+    <t>707 OverdueInterest</t>
+  </si>
+  <si>
+    <t>807 TotalOverdue</t>
+  </si>
+  <si>
+    <t>907 LoanDisbursementDateDisbursement</t>
+  </si>
+  <si>
+    <t>1007 ModeofReceipt</t>
+  </si>
+  <si>
+    <t>1107 PeriodMonths</t>
+  </si>
+  <si>
+    <t>1207 LoanRepaymentFrequency</t>
+  </si>
+  <si>
+    <t>1307 Purpose</t>
+  </si>
+  <si>
+    <t>308 PrincipalOutstandingIncludingArrears</t>
+  </si>
+  <si>
+    <t>408 PrincipalArrears</t>
+  </si>
+  <si>
+    <t>508 InterestRateAnnually</t>
+  </si>
+  <si>
+    <t>608 InterestPaid</t>
+  </si>
+  <si>
+    <t>708 OverdueInterest</t>
+  </si>
+  <si>
+    <t>808 TotalOverdue</t>
+  </si>
+  <si>
+    <t>908 LoanDisbursementDate</t>
+  </si>
+  <si>
+    <t>1008 ModeofReceipt</t>
+  </si>
+  <si>
+    <t>1108 PeriodMonths</t>
+  </si>
+  <si>
+    <t>1208 LoanRepaymentFrequency</t>
+  </si>
+  <si>
+    <t>1308 Purpose</t>
+  </si>
+  <si>
+    <t>613 BankName</t>
+  </si>
+  <si>
+    <t>713 TransactionNumber</t>
+  </si>
+  <si>
+    <t>813 ModeofReceipt</t>
+  </si>
+  <si>
+    <t>913 InterestRateAnnually</t>
+  </si>
+  <si>
+    <t>1013 AmountWithdrawn</t>
+  </si>
+  <si>
+    <t>1113 OriginalPeriodInMonths</t>
+  </si>
+  <si>
+    <t>1213 TotalOutstandingPeriod</t>
+  </si>
+  <si>
+    <t>1313 RemainingPeriod</t>
+  </si>
+  <si>
+    <t>1413 PrincipalRepaid</t>
+  </si>
+  <si>
+    <t>1513 PrincipalArrears</t>
+  </si>
+  <si>
+    <t>1613 InterestArrears</t>
+  </si>
+  <si>
+    <t>1713 RepaymentFrequency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1210,8 +1544,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1248,8 +1595,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1322,12 +1729,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1380,11 +1843,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1411,6 +1872,78 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1796,200 +2329,201 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A03593-CEAC-4FD9-A038-F5EE25925CE3}">
-  <dimension ref="A1:BI2"/>
+  <dimension ref="A1:BI9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="4" max="4" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="27" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:61" s="25" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="24" t="s">
+      <c r="S1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="T1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="24" t="s">
+      <c r="U1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="W1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="24" t="s">
+      <c r="X1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="24" t="s">
+      <c r="Y1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" s="24" t="s">
+      <c r="Z1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" s="24" t="s">
+      <c r="AA1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AB1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="24" t="s">
+      <c r="AC1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="24" t="s">
+      <c r="AD1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" s="24" t="s">
+      <c r="AE1" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="AF1" s="24" t="s">
+      <c r="AF1" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="AG1" s="24" t="s">
+      <c r="AG1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="AH1" s="24" t="s">
+      <c r="AH1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" s="24" t="s">
+      <c r="AI1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="AJ1" s="24" t="s">
+      <c r="AJ1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="AK1" s="24" t="s">
+      <c r="AK1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="AL1" s="24" t="s">
+      <c r="AL1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="AM1" s="25" t="s">
+      <c r="AM1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="AN1" s="25" t="s">
+      <c r="AN1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="AO1" s="25" t="s">
+      <c r="AO1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AP1" s="25" t="s">
+      <c r="AP1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="AQ1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="AR1" s="25" t="s">
+      <c r="AR1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AS1" s="25" t="s">
+      <c r="AS1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="AT1" s="25" t="s">
+      <c r="AT1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AU1" s="25" t="s">
+      <c r="AU1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="AV1" s="25" t="s">
+      <c r="AV1" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="AW1" s="25" t="s">
+      <c r="AW1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="AX1" s="25" t="s">
+      <c r="AX1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="AY1" s="25" t="s">
+      <c r="AY1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="AZ1" s="25" t="s">
+      <c r="AZ1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="BA1" s="25" t="s">
+      <c r="BA1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="BB1" s="25" t="s">
+      <c r="BB1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BC1" s="25" t="s">
+      <c r="BC1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="BD1" s="25" t="s">
+      <c r="BD1" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="BE1" s="25" t="s">
+      <c r="BE1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="BF1" s="25" t="s">
+      <c r="BF1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="BG1" s="25" t="s">
+      <c r="BG1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="BH1" s="25" t="s">
+      <c r="BH1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="BI1" s="26" t="s">
+      <c r="BI1" s="24" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1997,14 +2531,14 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C2" s="28" t="s">
+      <c r="B2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C2" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>237</v>
+      <c r="D2" t="s">
+        <v>266</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>147</v>
@@ -2012,47 +2546,47 @@
       <c r="F2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="1">
-        <v>1</v>
+      <c r="G2">
+        <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="P2" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="U2" s="1">
         <v>15</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="Z2" s="1">
         <v>300</v>
@@ -2067,31 +2601,31 @@
         <v>10</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>150</v>
       </c>
       <c r="AF2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="AJ2" s="1">
         <v>14</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AN2" s="1" t="s">
         <v>151</v>
@@ -2106,49 +2640,531 @@
         <v>153</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AS2" s="1" t="s">
         <v>154</v>
       </c>
       <c r="AT2" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AX2"/>
+      <c r="AY2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BC2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BE2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BF2" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BG2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>300</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>14</v>
+      </c>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP3" s="1">
+        <v>110049</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BH3" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1">
+        <v>15</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>300</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>14</v>
+      </c>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>110049</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AY4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AZ4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BC4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BD4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BE4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BF4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BG4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="BH4" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:61" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>110050</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>256</v>
       </c>
-      <c r="AU2" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BC2" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="BD2" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="BE2" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="BF2" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="BG2" s="1" t="s">
-        <v>158</v>
+      <c r="C6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" t="s">
+        <v>266</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2159,19 +3175,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCCD4E0-07FC-46A0-AF8C-3F93CADE071E}">
-  <dimension ref="A1:BH7"/>
+  <dimension ref="A1:BQ11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="13.21875" style="1"/>
+    <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="30.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
@@ -2353,18 +3369,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:60" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:69" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>146</v>
+      <c r="B2" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>235</v>
+        <v>160</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>161</v>
@@ -2429,7 +3445,7 @@
       <c r="Y2" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Z2" s="19" t="s">
+      <c r="Z2" s="18" t="s">
         <v>149</v>
       </c>
       <c r="AA2" s="16" t="s">
@@ -2441,8 +3457,6 @@
       <c r="AC2" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
       <c r="AF2" s="1" t="s">
         <v>174</v>
       </c>
@@ -2465,7 +3479,7 @@
         <v>110049</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="AN2" s="1" t="s">
         <v>184</v>
@@ -2485,7 +3499,6 @@
       <c r="AS2" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AT2" s="1"/>
       <c r="AU2" s="1" t="s">
         <v>149</v>
       </c>
@@ -2495,9 +3508,7 @@
       <c r="AW2" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="18" t="s">
+      <c r="AZ2" s="16" t="s">
         <v>189</v>
       </c>
       <c r="BA2" s="1" t="s">
@@ -2506,7 +3517,7 @@
       <c r="BB2" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BC2" s="18" t="s">
+      <c r="BC2" s="16" t="s">
         <v>192</v>
       </c>
       <c r="BD2" s="1" t="s">
@@ -2515,25 +3526,25 @@
       <c r="BE2" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BF2" s="20" t="s">
+      <c r="BF2" s="18" t="s">
         <v>227</v>
       </c>
       <c r="BG2" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:60" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:69" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>153</v>
+      <c r="B3" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>156</v>
+        <v>257</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>161</v>
@@ -2574,9 +3585,6 @@
       <c r="Q3" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
       <c r="V3" s="1" t="s">
         <v>174</v>
       </c>
@@ -2589,7 +3597,7 @@
       <c r="Y3" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="Z3" s="18" t="s">
         <v>149</v>
       </c>
       <c r="AA3" s="16" t="s">
@@ -2601,8 +3609,6 @@
       <c r="AC3" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
       <c r="AF3" s="1" t="s">
         <v>174</v>
       </c>
@@ -2625,7 +3631,7 @@
         <v>110050</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>156</v>
+        <v>257</v>
       </c>
       <c r="AN3" s="1" t="s">
         <v>199</v>
@@ -2654,7 +3660,7 @@
       <c r="AW3" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AZ3" s="18" t="s">
+      <c r="AZ3" s="16" t="s">
         <v>189</v>
       </c>
       <c r="BA3" s="1" t="s">
@@ -2663,7 +3669,7 @@
       <c r="BB3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BC3" s="18" t="s">
+      <c r="BC3" s="16" t="s">
         <v>192</v>
       </c>
       <c r="BD3" s="1" t="s">
@@ -2672,25 +3678,25 @@
       <c r="BE3" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="BF3" s="20" t="s">
+      <c r="BF3" s="18" t="s">
         <v>227</v>
       </c>
       <c r="BG3" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:60" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:69" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>153</v>
+      <c r="B4" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>160</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>157</v>
+        <v>258</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>161</v>
@@ -2755,7 +3761,7 @@
       <c r="Y4" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Z4" s="19" t="s">
+      <c r="Z4" s="18" t="s">
         <v>149</v>
       </c>
       <c r="AA4" s="16" t="s">
@@ -2767,8 +3773,6 @@
       <c r="AC4" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
       <c r="AF4" s="1" t="s">
         <v>174</v>
       </c>
@@ -2791,7 +3795,7 @@
         <v>110051</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>157</v>
+        <v>258</v>
       </c>
       <c r="AN4" s="1" t="s">
         <v>206</v>
@@ -2820,7 +3824,7 @@
       <c r="AW4" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AZ4" s="18" t="s">
+      <c r="AZ4" s="16" t="s">
         <v>189</v>
       </c>
       <c r="BA4" s="1" t="s">
@@ -2829,7 +3833,7 @@
       <c r="BB4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BC4" s="18" t="s">
+      <c r="BC4" s="16" t="s">
         <v>192</v>
       </c>
       <c r="BD4" s="1" t="s">
@@ -2838,19 +3842,19 @@
       <c r="BE4" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="BF4" s="20" t="s">
+      <c r="BF4" s="18" t="s">
         <v>227</v>
       </c>
       <c r="BG4" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:60" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:69" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>153</v>
+      <c r="B5" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>160</v>
@@ -2897,9 +3901,6 @@
       <c r="Q5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
       <c r="V5" s="1" t="s">
         <v>174</v>
       </c>
@@ -2912,7 +3913,7 @@
       <c r="Y5" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Z5" s="19" t="s">
+      <c r="Z5" s="18" t="s">
         <v>158</v>
       </c>
       <c r="AA5" s="16" t="s">
@@ -2924,8 +3925,6 @@
       <c r="AC5" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
       <c r="AF5" s="1" t="s">
         <v>174</v>
       </c>
@@ -2977,7 +3976,7 @@
       <c r="AW5" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AZ5" s="18" t="s">
+      <c r="AZ5" s="16" t="s">
         <v>189</v>
       </c>
       <c r="BA5" s="1" t="s">
@@ -2986,7 +3985,7 @@
       <c r="BB5" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BC5" s="18" t="s">
+      <c r="BC5" s="16" t="s">
         <v>192</v>
       </c>
       <c r="BD5" s="1" t="s">
@@ -2995,19 +3994,19 @@
       <c r="BE5" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="BF5" s="20" t="s">
+      <c r="BF5" s="18" t="s">
         <v>227</v>
       </c>
       <c r="BG5" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:60" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:69" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>153</v>
+      <c r="B6" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>160</v>
@@ -3078,7 +4077,7 @@
       <c r="Y6" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Z6" s="19" t="s">
+      <c r="Z6" s="18" t="s">
         <v>158</v>
       </c>
       <c r="AA6" s="16" t="s">
@@ -3090,8 +4089,6 @@
       <c r="AC6" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
       <c r="AF6" s="1" t="s">
         <v>174</v>
       </c>
@@ -3143,7 +4140,7 @@
       <c r="AW6" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AZ6" s="18" t="s">
+      <c r="AZ6" s="16" t="s">
         <v>189</v>
       </c>
       <c r="BA6" s="1" t="s">
@@ -3152,7 +4149,7 @@
       <c r="BB6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BC6" s="18" t="s">
+      <c r="BC6" s="16" t="s">
         <v>192</v>
       </c>
       <c r="BD6" s="1" t="s">
@@ -3161,19 +4158,19 @@
       <c r="BE6" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="BF6" s="20" t="s">
+      <c r="BF6" s="18" t="s">
         <v>227</v>
       </c>
       <c r="BG6" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:60" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:69" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>153</v>
+      <c r="B7" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>160</v>
@@ -3244,7 +4241,7 @@
       <c r="Y7" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Z7" s="19" t="s">
+      <c r="Z7" s="18" t="s">
         <v>158</v>
       </c>
       <c r="AA7" s="16" t="s">
@@ -3256,8 +4253,6 @@
       <c r="AC7" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
       <c r="AF7" s="1" t="s">
         <v>174</v>
       </c>
@@ -3309,7 +4304,7 @@
       <c r="AW7" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AZ7" s="18" t="s">
+      <c r="AZ7" s="16" t="s">
         <v>189</v>
       </c>
       <c r="BA7" s="1" t="s">
@@ -3318,7 +4313,7 @@
       <c r="BB7" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BC7" s="18" t="s">
+      <c r="BC7" s="16" t="s">
         <v>192</v>
       </c>
       <c r="BD7" s="1" t="s">
@@ -3327,11 +4322,241 @@
       <c r="BE7" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="BF7" s="20" t="s">
+      <c r="BF7" s="18" t="s">
         <v>227</v>
       </c>
       <c r="BG7" s="1" t="s">
         <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="1">
+        <v>24</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y8" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z8" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA8" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB8" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="AC8" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>110051</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AO8" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ8" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS8" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AV8" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AW8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AZ8" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="BA8" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="BB8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BC8" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="BD8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BE8" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="BF8" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="BG8" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="BQ8" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="K9" s="17"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AM9" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO9" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP9" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ9" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AR9" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AZ9" s="16"/>
+      <c r="BC9" s="16"/>
+      <c r="BF9" s="18"/>
+    </row>
+    <row r="10" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -3436,4 +4661,791 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B057BC25-0B06-47D9-9B75-89C2A0553E69}">
+  <dimension ref="A1:DD87"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.21875" style="29" customWidth="1"/>
+    <col min="2" max="3" width="19.21875" style="29"/>
+    <col min="4" max="16384" width="19.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:108" s="41" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="M1" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>326</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>328</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>330</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="U1" s="31" t="s">
+        <v>332</v>
+      </c>
+      <c r="V1" s="31" t="s">
+        <v>333</v>
+      </c>
+      <c r="W1" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="X1" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="Y1" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z1" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="AA1" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB1" s="47" t="s">
+        <v>336</v>
+      </c>
+      <c r="AC1" s="47" t="s">
+        <v>337</v>
+      </c>
+      <c r="AD1" s="47" t="s">
+        <v>338</v>
+      </c>
+      <c r="AE1" s="47" t="s">
+        <v>339</v>
+      </c>
+      <c r="AF1" s="47" t="s">
+        <v>340</v>
+      </c>
+      <c r="AG1" s="47" t="s">
+        <v>341</v>
+      </c>
+      <c r="AH1" s="47" t="s">
+        <v>342</v>
+      </c>
+      <c r="AI1" s="47" t="s">
+        <v>343</v>
+      </c>
+      <c r="AJ1" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="AK1" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="AL1" s="47" t="s">
+        <v>346</v>
+      </c>
+      <c r="AM1" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="AN1" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="AO1" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="AP1" s="48" t="s">
+        <v>347</v>
+      </c>
+      <c r="AQ1" s="48" t="s">
+        <v>348</v>
+      </c>
+      <c r="AR1" s="48" t="s">
+        <v>349</v>
+      </c>
+      <c r="AS1" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="AT1" s="48" t="s">
+        <v>351</v>
+      </c>
+      <c r="AU1" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="AV1" s="48" t="s">
+        <v>353</v>
+      </c>
+      <c r="AW1" s="48" t="s">
+        <v>354</v>
+      </c>
+      <c r="AX1" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="AY1" s="48" t="s">
+        <v>356</v>
+      </c>
+      <c r="AZ1" s="48" t="s">
+        <v>357</v>
+      </c>
+      <c r="BA1" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="BB1" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="BC1" s="43" t="s">
+        <v>288</v>
+      </c>
+      <c r="BD1" s="43" t="s">
+        <v>289</v>
+      </c>
+      <c r="BE1" s="43" t="s">
+        <v>290</v>
+      </c>
+      <c r="BF1" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="BG1" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="BH1" s="44" t="s">
+        <v>293</v>
+      </c>
+      <c r="BI1" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="BJ1" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="BK1" s="41" t="s">
+        <v>296</v>
+      </c>
+      <c r="BL1" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="BM1" s="41" t="s">
+        <v>298</v>
+      </c>
+      <c r="BN1" s="41" t="s">
+        <v>299</v>
+      </c>
+      <c r="BO1" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="BP1" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="BQ1" s="47" t="s">
+        <v>358</v>
+      </c>
+      <c r="BR1" s="47" t="s">
+        <v>359</v>
+      </c>
+      <c r="BS1" s="47" t="s">
+        <v>360</v>
+      </c>
+      <c r="BT1" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="BU1" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="BV1" s="47" t="s">
+        <v>363</v>
+      </c>
+      <c r="BW1" s="47" t="s">
+        <v>364</v>
+      </c>
+      <c r="BX1" s="47" t="s">
+        <v>365</v>
+      </c>
+      <c r="BY1" s="47" t="s">
+        <v>366</v>
+      </c>
+      <c r="BZ1" s="47" t="s">
+        <v>367</v>
+      </c>
+      <c r="CA1" s="47" t="s">
+        <v>368</v>
+      </c>
+      <c r="CB1" s="47" t="s">
+        <v>369</v>
+      </c>
+      <c r="CC1" s="41" t="s">
+        <v>302</v>
+      </c>
+      <c r="CD1" s="45" t="s">
+        <v>303</v>
+      </c>
+      <c r="CE1" s="45" t="s">
+        <v>304</v>
+      </c>
+      <c r="CF1" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="CG1" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="CH1" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="CI1" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="CJ1" s="46" t="s">
+        <v>309</v>
+      </c>
+      <c r="CK1" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="CL1" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="CM1" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="CN1" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="CO1" s="34" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="1">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F2" s="1">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1">
+        <v>200</v>
+      </c>
+      <c r="H2" s="1">
+        <v>200</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1">
+        <v>100</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="L2" s="1">
+        <v>500</v>
+      </c>
+      <c r="M2" s="1">
+        <v>200</v>
+      </c>
+      <c r="O2" s="1">
+        <v>50</v>
+      </c>
+      <c r="P2" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>10</v>
+      </c>
+      <c r="R2" s="1">
+        <v>10</v>
+      </c>
+      <c r="S2" s="1">
+        <v>60</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="V2" s="1">
+        <v>10</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>500</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>200</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>500</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>200</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>50</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>60</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>200</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>100</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>500</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:108" s="50" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
+      <c r="AM3" s="49"/>
+      <c r="AN3" s="49"/>
+      <c r="AO3" s="49"/>
+      <c r="AP3" s="49"/>
+      <c r="BA3" s="49"/>
+      <c r="BB3" s="49"/>
+      <c r="BC3" s="49"/>
+      <c r="BD3" s="49"/>
+      <c r="BE3" s="49"/>
+      <c r="BF3" s="49"/>
+      <c r="BG3" s="49"/>
+      <c r="BH3" s="49"/>
+      <c r="BI3" s="49"/>
+      <c r="BJ3" s="49"/>
+      <c r="BK3" s="49"/>
+      <c r="BL3" s="49"/>
+      <c r="BM3" s="49"/>
+      <c r="BN3" s="49"/>
+      <c r="BO3" s="49"/>
+      <c r="BP3" s="49"/>
+      <c r="BR3" s="49"/>
+      <c r="BS3" s="49"/>
+      <c r="CD3" s="49"/>
+      <c r="CE3" s="49"/>
+      <c r="CF3" s="49"/>
+      <c r="CG3" s="49"/>
+      <c r="CH3" s="49"/>
+      <c r="CI3" s="49"/>
+      <c r="CJ3" s="49"/>
+      <c r="CK3" s="49"/>
+      <c r="CL3" s="49"/>
+      <c r="CM3" s="49"/>
+      <c r="CN3" s="49"/>
+      <c r="CO3" s="49"/>
+      <c r="CP3" s="49"/>
+      <c r="CQ3" s="49"/>
+      <c r="CR3" s="49"/>
+      <c r="CS3" s="51"/>
+      <c r="CU3" s="49"/>
+      <c r="CV3" s="49"/>
+      <c r="CW3" s="49"/>
+      <c r="CX3" s="49"/>
+      <c r="CY3" s="49"/>
+      <c r="CZ3" s="49"/>
+      <c r="DA3" s="49"/>
+      <c r="DB3" s="49"/>
+      <c r="DC3" s="49"/>
+      <c r="DD3" s="49"/>
+    </row>
+    <row r="4" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A4" s="28"/>
+    </row>
+    <row r="5" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A5" s="30"/>
+    </row>
+    <row r="6" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A6" s="30"/>
+    </row>
+    <row r="7" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
+    </row>
+    <row r="8" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A8" s="30"/>
+    </row>
+    <row r="9" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
+    </row>
+    <row r="10" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A10" s="30"/>
+    </row>
+    <row r="11" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+    </row>
+    <row r="12" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+    </row>
+    <row r="13" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
+    </row>
+    <row r="14" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+    </row>
+    <row r="15" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+    </row>
+    <row r="16" spans="1:108" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="30"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="30"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="30"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="30"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="30"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="30"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="30"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="30"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="30"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="30"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="30"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="30"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="30"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="30"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="30"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="30"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="30"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="30"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="30"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="30"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="30"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="30"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="30"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="30"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="30"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="30"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="30"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="30"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="30"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="30"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="30"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="30"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="30"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="30"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="30"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="30"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="30"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="30"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="30"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="30"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="30"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="30"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="30"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="30"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="30"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="30"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="30"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="30"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="30"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="30"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="30"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="30"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="30"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="30"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="30"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="30"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="30"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="30"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="30"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="30"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="30"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="30"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="30"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="30"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="30"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="30"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="30"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>